<commit_message>
primer grafico ya echo
</commit_message>
<xml_diff>
--- a/Documentation/Comparador Tabla de NDout con graficos.xlsx
+++ b/Documentation/Comparador Tabla de NDout con graficos.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="8910" windowHeight="7080"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Gráfico3" sheetId="6" r:id="rId1"/>
+    <sheet name="RAW Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="33">
   <si>
     <t>EXP</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>Variacion de tension</t>
   </si>
 </sst>
 </file>
@@ -285,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -482,6 +486,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,6 +499,553 @@
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RAW Data'!$A$5:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>menos 8mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="114300" prst="artDeco"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.8875999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5506000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9775</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6516999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$T$5:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.4673743365594665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.517327505463627</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1027162035591642</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5335622853574868</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6153605994380174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.321261317514836</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.394005619731491</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RAW Data'!$A$22:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>menos 5mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="101600" prst="riblet"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$D$22:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0561999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9438000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3707999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.7639999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.325799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.667000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$T$22:$T$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.7728374846490473</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8389646377176758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9649526088736327</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8057121264603051</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5312844412255542</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.338382088988258</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.657335390622539</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RAW Data'!$I$5:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mas 5mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="152400" h="50800" prst="softRound"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$L$5:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9100999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0336999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9326000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.610999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$X$5:$X$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1457.3688711516534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>801.41106043329523</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5567.930444697834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1355.3734321550744</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2534.6493728620294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56574.743443557585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9634.5014245014245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RAW Data'!$I$22:$I$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mas 8mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FFFF00"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT/>
+              </a:sp3d>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$L$22:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9663000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7079000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3257999999999992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.055999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.262999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RAW Data'!$X$22:$X$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3612.5364431486878</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>835.21400778210125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14912.490272373543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1250.3891050583657</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6383.735408560311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155001.16731517512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25999.922178988327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="67133824"/>
+        <c:axId val="67135360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67133824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67135360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="67135360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67133824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="-97414"/>
+    <xdr:ext cx="8680739" cy="6396904"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O113"/>
+  <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -801,9 +1353,14 @@
     <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="14" width="17.5703125" customWidth="1"/>
     <col min="15" max="15" width="5.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:24">
       <c r="A1" s="107" t="s">
         <v>21</v>
       </c>
@@ -822,7 +1379,7 @@
       <c r="N1" s="107"/>
       <c r="O1" s="107"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15">
+    <row r="2" spans="1:24" s="1" customFormat="1" ht="15">
       <c r="A2" s="105" t="s">
         <v>14</v>
       </c>
@@ -867,7 +1424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="15">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="15">
       <c r="A3" s="106"/>
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
@@ -883,8 +1440,11 @@
       <c r="M3" s="94"/>
       <c r="N3" s="94"/>
       <c r="O3" s="92"/>
-    </row>
-    <row r="4" spans="1:15" s="2" customFormat="1">
+      <c r="T3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="2" customFormat="1">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -900,8 +1460,16 @@
       <c r="M4" s="43"/>
       <c r="N4" s="43"/>
       <c r="O4" s="44"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1">
+      <c r="Q4" s="27"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="97" t="s">
         <v>17</v>
       </c>
@@ -947,8 +1515,34 @@
       <c r="O5" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="Q5" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5">
+        <f>(ABS(E5-F5)/E5)*100</f>
+        <v>1.4673743365594665</v>
+      </c>
+      <c r="U5" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="108">
+        <f>(ABS(M5-N5)/M5)*100</f>
+        <v>1457.3688711516534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="97"/>
       <c r="B6" s="12"/>
       <c r="C6" s="6" t="s">
@@ -986,8 +1580,26 @@
       <c r="O6" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="Q6" s="97"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" ref="T6:T36" si="0">(ABS(E6-F6)/E6)*100</f>
+        <v>1.517327505463627</v>
+      </c>
+      <c r="U6" s="101"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6" s="108">
+        <f t="shared" ref="X6:X36" si="1">(ABS(M6-N6)/M6)*100</f>
+        <v>801.41106043329523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="97"/>
       <c r="B7" s="12"/>
       <c r="C7" s="6" t="s">
@@ -1025,8 +1637,26 @@
       <c r="O7" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="Q7" s="97"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="0"/>
+        <v>7.1027162035591642</v>
+      </c>
+      <c r="U7" s="101"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="108">
+        <f t="shared" si="1"/>
+        <v>5567.930444697834</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="97"/>
       <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
@@ -1064,8 +1694,26 @@
       <c r="O8" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="Q8" s="97"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="0"/>
+        <v>7.5335622853574868</v>
+      </c>
+      <c r="U8" s="101"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="108">
+        <f t="shared" si="1"/>
+        <v>1355.3734321550744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="97"/>
       <c r="B9" s="12"/>
       <c r="C9" s="6" t="s">
@@ -1103,8 +1751,26 @@
       <c r="O9" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="Q9" s="97"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="0"/>
+        <v>3.6153605994380174</v>
+      </c>
+      <c r="U9" s="101"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="108">
+        <f t="shared" si="1"/>
+        <v>2534.6493728620294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="97"/>
       <c r="B10" s="12"/>
       <c r="C10" s="6" t="s">
@@ -1142,8 +1808,26 @@
       <c r="O10" s="86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="Q10" s="97"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="0"/>
+        <v>17.321261317514836</v>
+      </c>
+      <c r="U10" s="101"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="X10" s="108">
+        <f t="shared" si="1"/>
+        <v>56574.743443557585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="97"/>
       <c r="B11" s="14"/>
       <c r="C11" s="8" t="s">
@@ -1181,8 +1865,26 @@
       <c r="O11" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="Q11" s="97"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="0"/>
+        <v>16.394005619731491</v>
+      </c>
+      <c r="U11" s="101"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X11" s="108">
+        <f t="shared" si="1"/>
+        <v>9634.5014245014245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="97"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1198,8 +1900,16 @@
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="18"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="Q12" s="97"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="108"/>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="97"/>
       <c r="B13" s="10" t="s">
         <v>7</v>
@@ -1241,8 +1951,30 @@
       <c r="O13" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="Q13" s="97"/>
+      <c r="R13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="0"/>
+        <v>1.4985950671245722</v>
+      </c>
+      <c r="U13" s="101"/>
+      <c r="V13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="108">
+        <f t="shared" si="1"/>
+        <v>1485.7468643101481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="97"/>
       <c r="B14" s="12"/>
       <c r="C14" s="6" t="s">
@@ -1280,8 +2012,26 @@
       <c r="O14" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="Q14" s="97"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5079612862941065</v>
+      </c>
+      <c r="U14" s="101"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="X14" s="108">
+        <f t="shared" si="1"/>
+        <v>806.84150513112888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" s="97"/>
       <c r="B15" s="12"/>
       <c r="C15" s="6" t="s">
@@ -1319,8 +2069,26 @@
       <c r="O15" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="Q15" s="97"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="5">
+        <f t="shared" si="0"/>
+        <v>7.1776459569153852</v>
+      </c>
+      <c r="U15" s="101"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" s="108">
+        <f t="shared" si="1"/>
+        <v>5788.9680729760548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="97"/>
       <c r="B16" s="12"/>
       <c r="C16" s="6" t="s">
@@ -1358,8 +2126,26 @@
       <c r="O16" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="Q16" s="97"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="5">
+        <f t="shared" si="0"/>
+        <v>7.7146425226350335</v>
+      </c>
+      <c r="U16" s="101"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="108">
+        <f t="shared" si="1"/>
+        <v>1354.0906499429877</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17" s="97"/>
       <c r="B17" s="12"/>
       <c r="C17" s="6" t="s">
@@ -1397,8 +2183,26 @@
       <c r="O17" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="Q17" s="97"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17" s="5">
+        <f t="shared" si="0"/>
+        <v>4.6831095847642805</v>
+      </c>
+      <c r="U17" s="101"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" s="108">
+        <f t="shared" si="1"/>
+        <v>3180.7012542759408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" s="97"/>
       <c r="B18" s="12"/>
       <c r="C18" s="6" t="s">
@@ -1436,8 +2240,26 @@
       <c r="O18" s="86" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18" s="97"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T18" s="5">
+        <f t="shared" si="0"/>
+        <v>15.472994068061194</v>
+      </c>
+      <c r="U18" s="101"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="X18" s="108">
+        <f t="shared" si="1"/>
+        <v>56751.482326111749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19" s="97"/>
       <c r="B19" s="14"/>
       <c r="C19" s="8" t="s">
@@ -1475,8 +2297,26 @@
       <c r="O19" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="Q19" s="97"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="0"/>
+        <v>16.781142678738671</v>
+      </c>
+      <c r="U19" s="101"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X19" s="108">
+        <f t="shared" si="1"/>
+        <v>9638.803418803418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" s="98"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1492,8 +2332,16 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="20"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="Q20" s="98"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="102"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="108"/>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" s="30"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
@@ -1509,8 +2357,16 @@
       <c r="M21" s="46"/>
       <c r="N21" s="46"/>
       <c r="O21" s="47"/>
-    </row>
-    <row r="22" spans="1:15" ht="16.5" customHeight="1">
+      <c r="Q21" s="30"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="108"/>
+    </row>
+    <row r="22" spans="1:24" ht="16.5" customHeight="1">
       <c r="A22" s="99" t="s">
         <v>18</v>
       </c>
@@ -1556,8 +2412,34 @@
       <c r="O22" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="Q22" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="T22" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7728374846490473</v>
+      </c>
+      <c r="U22" s="103" t="s">
+        <v>20</v>
+      </c>
+      <c r="V22" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="X22" s="108">
+        <f t="shared" si="1"/>
+        <v>3612.5364431486878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23" s="99"/>
       <c r="B23" s="36"/>
       <c r="C23" s="37" t="s">
@@ -1595,8 +2477,26 @@
       <c r="O23" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="Q23" s="99"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8389646377176758</v>
+      </c>
+      <c r="U23" s="103"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="X23" s="108">
+        <f t="shared" si="1"/>
+        <v>835.21400778210125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24" s="99"/>
       <c r="B24" s="36"/>
       <c r="C24" s="37" t="s">
@@ -1634,8 +2534,26 @@
       <c r="O24" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="Q24" s="99"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="T24" s="5">
+        <f t="shared" si="0"/>
+        <v>8.9649526088736327</v>
+      </c>
+      <c r="U24" s="103"/>
+      <c r="V24" s="51"/>
+      <c r="W24" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="108">
+        <f t="shared" si="1"/>
+        <v>14912.490272373543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25" s="99"/>
       <c r="B25" s="36"/>
       <c r="C25" s="37" t="s">
@@ -1673,8 +2591,26 @@
       <c r="O25" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="Q25" s="99"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="T25" s="5">
+        <f t="shared" si="0"/>
+        <v>9.8057121264603051</v>
+      </c>
+      <c r="U25" s="103"/>
+      <c r="V25" s="51"/>
+      <c r="W25" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X25" s="108">
+        <f t="shared" si="1"/>
+        <v>1250.3891050583657</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26" s="99"/>
       <c r="B26" s="36"/>
       <c r="C26" s="37" t="s">
@@ -1712,8 +2648,26 @@
       <c r="O26" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="Q26" s="99"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="T26" s="5">
+        <f t="shared" si="0"/>
+        <v>4.5312844412255542</v>
+      </c>
+      <c r="U26" s="103"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="X26" s="108">
+        <f t="shared" si="1"/>
+        <v>6383.735408560311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" s="99"/>
       <c r="B27" s="36"/>
       <c r="C27" s="37" t="s">
@@ -1751,8 +2705,26 @@
       <c r="O27" s="81" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="Q27" s="99"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="T27" s="5">
+        <f t="shared" si="0"/>
+        <v>22.338382088988258</v>
+      </c>
+      <c r="U27" s="103"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="X27" s="108">
+        <f t="shared" si="1"/>
+        <v>155001.16731517512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" s="99"/>
       <c r="B28" s="39"/>
       <c r="C28" s="40" t="s">
@@ -1790,8 +2762,26 @@
       <c r="O28" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="Q28" s="99"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="T28" s="5">
+        <f t="shared" si="0"/>
+        <v>25.657335390622539</v>
+      </c>
+      <c r="U28" s="103"/>
+      <c r="V28" s="56"/>
+      <c r="W28" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="X28" s="108">
+        <f t="shared" si="1"/>
+        <v>25999.922178988327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" s="99"/>
       <c r="B29" s="37"/>
       <c r="C29" s="37"/>
@@ -1807,8 +2797,16 @@
       <c r="M29" s="52"/>
       <c r="N29" s="52"/>
       <c r="O29" s="50"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="Q29" s="99"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="103"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="108"/>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" s="99"/>
       <c r="B30" s="33" t="s">
         <v>7</v>
@@ -1850,8 +2848,30 @@
       <c r="O30" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="Q30" s="99"/>
+      <c r="R30" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="S30" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8137733413105734</v>
+      </c>
+      <c r="U30" s="103"/>
+      <c r="V30" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="W30" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="X30" s="108">
+        <f t="shared" si="1"/>
+        <v>3813.4305150631681</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" s="99"/>
       <c r="B31" s="36"/>
       <c r="C31" s="37" t="s">
@@ -1889,8 +2909,26 @@
       <c r="O31" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="Q31" s="99"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="T31" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8641559341247644</v>
+      </c>
+      <c r="U31" s="103"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="X31" s="108">
+        <f t="shared" si="1"/>
+        <v>851.82879377431925</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32" s="99"/>
       <c r="B32" s="36"/>
       <c r="C32" s="37" t="s">
@@ -1928,8 +2966,26 @@
       <c r="O32" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="Q32" s="99"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="T32" s="5">
+        <f t="shared" si="0"/>
+        <v>8.9366124004156511</v>
+      </c>
+      <c r="U32" s="103"/>
+      <c r="V32" s="51"/>
+      <c r="W32" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="X32" s="108">
+        <f t="shared" si="1"/>
+        <v>16017.237354085606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" s="99"/>
       <c r="B33" s="36"/>
       <c r="C33" s="37" t="s">
@@ -1967,8 +3023,26 @@
       <c r="O33" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="Q33" s="99"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="T33" s="5">
+        <f t="shared" si="0"/>
+        <v>10.177283748464903</v>
+      </c>
+      <c r="U33" s="103"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X33" s="108">
+        <f t="shared" si="1"/>
+        <v>1252.9182879377431</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" s="99"/>
       <c r="B34" s="36"/>
       <c r="C34" s="37" t="s">
@@ -2006,8 +3080,26 @@
       <c r="O34" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="Q34" s="99"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="T34" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6806373397991026</v>
+      </c>
+      <c r="U34" s="103"/>
+      <c r="V34" s="51"/>
+      <c r="W34" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="X34" s="108">
+        <f t="shared" si="1"/>
+        <v>7907.3929961089489</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35" s="99"/>
       <c r="B35" s="36"/>
       <c r="C35" s="37" t="s">
@@ -2045,8 +3137,26 @@
       <c r="O35" s="81" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="Q35" s="99"/>
+      <c r="R35" s="36"/>
+      <c r="S35" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="T35" s="5">
+        <f t="shared" si="0"/>
+        <v>20.899329281733159</v>
+      </c>
+      <c r="U35" s="103"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="X35" s="108">
+        <f t="shared" si="1"/>
+        <v>154915.56420233464</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" s="99"/>
       <c r="B36" s="39"/>
       <c r="C36" s="40" t="s">
@@ -2084,8 +3194,26 @@
       <c r="O36" s="50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="Q36" s="99"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="T36" s="5">
+        <f t="shared" si="0"/>
+        <v>27.571873917561479</v>
+      </c>
+      <c r="U36" s="103"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="X36" s="108">
+        <f t="shared" si="1"/>
+        <v>26162.957198443582</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
       <c r="A37" s="100"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -2101,9 +3229,17 @@
       <c r="M37" s="57"/>
       <c r="N37" s="57"/>
       <c r="O37" s="58"/>
-    </row>
-    <row r="38" spans="1:15" ht="17.25" customHeight="1"/>
-    <row r="39" spans="1:15">
+      <c r="Q37" s="100"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="40"/>
+      <c r="U37" s="104"/>
+      <c r="V37" s="57"/>
+      <c r="W37" s="57"/>
+      <c r="X37" s="57"/>
+    </row>
+    <row r="38" spans="1:24" ht="17.25" customHeight="1"/>
+    <row r="39" spans="1:24">
       <c r="A39" s="107" t="s">
         <v>22</v>
       </c>
@@ -2122,7 +3258,7 @@
       <c r="N39" s="107"/>
       <c r="O39" s="107"/>
     </row>
-    <row r="40" spans="1:15" ht="15">
+    <row r="40" spans="1:24" ht="15">
       <c r="A40" s="105" t="s">
         <v>14</v>
       </c>
@@ -2167,7 +3303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15">
+    <row r="41" spans="1:24" ht="15">
       <c r="A41" s="106"/>
       <c r="B41" s="94"/>
       <c r="C41" s="94"/>
@@ -2184,7 +3320,7 @@
       <c r="N41" s="94"/>
       <c r="O41" s="92"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:24">
       <c r="A42" s="27"/>
       <c r="B42" s="28"/>
       <c r="C42" s="28"/>
@@ -2201,7 +3337,7 @@
       <c r="N42" s="43"/>
       <c r="O42" s="44"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:24">
       <c r="A43" s="97" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +3384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:24">
       <c r="A44" s="97"/>
       <c r="B44" s="12"/>
       <c r="C44" s="6" t="s">
@@ -2287,7 +3423,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:24">
       <c r="A45" s="97"/>
       <c r="B45" s="12"/>
       <c r="C45" s="6" t="s">
@@ -2326,7 +3462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:24">
       <c r="A46" s="97"/>
       <c r="B46" s="12"/>
       <c r="C46" s="6" t="s">
@@ -2365,7 +3501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:24">
       <c r="A47" s="97"/>
       <c r="B47" s="12"/>
       <c r="C47" s="6" t="s">
@@ -2404,7 +3540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:24">
       <c r="A48" s="97"/>
       <c r="B48" s="12"/>
       <c r="C48" s="6" t="s">
@@ -4254,7 +5390,11 @@
       <c r="O113" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="61">
+    <mergeCell ref="Q5:Q20"/>
+    <mergeCell ref="U5:U20"/>
+    <mergeCell ref="Q22:Q37"/>
+    <mergeCell ref="U22:U37"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A39:O39"/>
     <mergeCell ref="A77:O77"/>

</xml_diff>